<commit_message>
adding CC0 license with permission from Stephen Kramer
</commit_message>
<xml_diff>
--- a/Covid19_Projects_from_YouTube.xlsx
+++ b/Covid19_Projects_from_YouTube.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertread/PubInv/covid19-vent-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{730697E1-C360-4A41-A3D8-3211A43F7ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5A5A4-4F71-EB4B-8FF6-14796D1D5321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1140" windowWidth="38880" windowHeight="21320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="441">
   <si>
     <t>Marco Mascorro</t>
   </si>
@@ -1358,6 +1358,12 @@
   </si>
   <si>
     <t>https://www.youtube.com/redirect?q=https%3A%2F%2Fdrive.google.com%2Fopen%3Fid%3D1SBuUAbx5IWoYnzWg3vVrB7b8yaZ0vjuG&amp;v=dCnaK7_GXFU&amp;event=video_description&amp;redir_token=8jOJq9EBN5x0kHgHU-_Io0PZneN8MTU4NTY5MzIxMEAxNTg1NjA2ODEw</t>
+  </si>
+  <si>
+    <t>This spreadshee was created by Stephen Kramer, March 30, 2020.</t>
+  </si>
+  <si>
+    <t>Licensed with CC0 1.0 Universal</t>
   </si>
 </sst>
 </file>
@@ -2372,11 +2378,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABACE4E4-1789-4929-BA04-084550DEC681}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="21"/>
@@ -4259,6 +4265,16 @@
       </c>
       <c r="I127" s="8" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" ht="33">
+      <c r="B130" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" s="8" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -4485,8 +4501,9 @@
     <hyperlink ref="E124" r:id="rId220" display="https://www.youtube.com/channel/UCKi3uN6-_dz66TWRkHFzdhQ" xr:uid="{6E9C2890-4FEB-4739-A649-0D6B8C46C512}"/>
     <hyperlink ref="E126" r:id="rId221" display="https://www.youtube.com/channel/UCjl12fpLY_P9RO4FeEHzrcQ" xr:uid="{F21253EE-7E7A-4462-9741-FECDE7677481}"/>
     <hyperlink ref="C126" r:id="rId222" xr:uid="{8A0B8481-DD90-4E4C-932A-BDCD2784AF3F}"/>
+    <hyperlink ref="B131" r:id="rId223" xr:uid="{54380550-74FB-3943-BD88-FF9D3C849212}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId223"/>
+  <pageSetup orientation="portrait" r:id="rId224"/>
 </worksheet>
 </file>
</xml_diff>